<commit_message>
Added mtry Tuning and Log Loss
</commit_message>
<xml_diff>
--- a/Heart Disease Classifier Results.xlsx
+++ b/Heart Disease Classifier Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\One-Drive\OneDrive - Tredence\Personal Projects\Heart Disease Classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC435DEA-2A03-45D8-AC2C-4A0DA9886CFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{FC435DEA-2A03-45D8-AC2C-4A0DA9886CFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E1A7E39D-F6BA-4C7A-A5F2-1B72986282DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,11 @@
     <sheet name="All Data Prediction" sheetId="15" r:id="rId2"/>
     <sheet name="Feature Importance" sheetId="10" r:id="rId3"/>
     <sheet name="ROC Curve" sheetId="11" r:id="rId4"/>
-    <sheet name="Number of Nodes" sheetId="12" r:id="rId5"/>
-    <sheet name="Optimal Trees" sheetId="13" r:id="rId6"/>
-    <sheet name="Correlogram" sheetId="14" r:id="rId7"/>
+    <sheet name="Log Loss" sheetId="17" r:id="rId5"/>
+    <sheet name="Number of Nodes" sheetId="12" r:id="rId6"/>
+    <sheet name="Optimal Trees" sheetId="13" r:id="rId7"/>
+    <sheet name="Optimal mtry" sheetId="16" r:id="rId8"/>
+    <sheet name="Correlogram" sheetId="14" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Feature Importance'!$B$3:$C$3</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Predicted</t>
   </si>
@@ -145,6 +147,15 @@
   </si>
   <si>
     <t>Model Results and Accuracy - All Data</t>
+  </si>
+  <si>
+    <t>Optimize mtry - Number of variables available for splitting at each node</t>
+  </si>
+  <si>
+    <t>Log Loss</t>
+  </si>
+  <si>
+    <t>Global Log Loss:</t>
   </si>
 </sst>
 </file>
@@ -242,7 +253,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,6 +293,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1428,6 +1440,61 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48491E89-A3D4-4315-B683-0DD7E1721F4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247649" y="952501"/>
+          <a:ext cx="5591176" cy="4193382"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -1479,7 +1546,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1534,7 +1601,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{445DE97C-A510-44B5-8BBA-253AD7C2B2A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="571500"/>
+          <a:ext cx="4543426" cy="4543426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2665,6 +2787,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58227D-4EA5-4D77-8CA5-CB774D8591AF}">
+  <dimension ref="B1:K3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17">
+        <v>0.43733630000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7679A83C-5B12-48FB-A918-E50296CD2744}">
   <dimension ref="B1:K2"/>
   <sheetViews>
@@ -2696,7 +2859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04DAD6B-DCB0-4EB1-AC25-F324AD606248}">
   <dimension ref="B1:K2"/>
   <sheetViews>
@@ -2728,7 +2891,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D0B26A-827E-429B-B1A2-377999121AEC}">
+  <dimension ref="B1:K2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA85811-B04A-4AC5-B4E7-9C8CD1534C78}">
   <dimension ref="B1:K2"/>
   <sheetViews>
@@ -2950,14 +3146,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A562643A-DE27-4DFC-9CB1-F40791435515}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="241d78fe-eaa9-4719-83de-4d7c348c932d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>